<commit_message>
reformatted demo data to work with close of #46
Also minor changes to demo.py itself for the same reaon
</commit_message>
<xml_diff>
--- a/scenarios-examples/demo/data/factories/cementFactory_mysterious.xlsx
+++ b/scenarios-examples/demo/data/factories/cementFactory_mysterious.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\demo\factories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/scenarios-examples/demo/data/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435D76B9-1E49-E04F-9D50-E92A384A1807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2205" windowWidth="27645" windowHeight="16545" activeTab="1"/>
+    <workbookView xWindow="1160" yWindow="2200" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="cementFactoryChains" localSheetId="0">'Chain List'!$A$1:$D$3</definedName>
     <definedName name="cementFlow" localSheetId="1">'Cement Chain'!$A$1:$C$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,8 +30,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="cementFactoryChains" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="cementFactoryChains" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/cementFactoryChains.tsv" thousands=" ">
       <textFields count="4">
         <textField/>
@@ -40,7 +41,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="cementFlow" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="cementFlow" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/cementFlow.tsv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -100,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -151,11 +152,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cementFactoryChains" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cementFactoryChains" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cementFlow" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cementFlow" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -454,23 +455,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -510,21 +511,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -535,7 +536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>

</xml_diff>